<commit_message>
Update link to privacy policy document
</commit_message>
<xml_diff>
--- a/inst/formr/bvq-1.0.0/bvq_03_consent.xlsx
+++ b/inst/formr/bvq-1.0.0/bvq_03_consent.xlsx
@@ -93,19 +93,19 @@
     <t xml:space="preserve">link_catalan</t>
   </si>
   <si>
-    <t xml:space="preserve">**[Document de política de privacitat](https://drive.google.com/a/upf.edu/file/d/1kVoS9UP_WuHszbi8UJH9yXMWYg5gnJqk/view?usp=sharing)**</t>
+    <t xml:space="preserve">**[Política de privacitat](https://www.upf.edu/web/cbclab/politica-privacitat)**</t>
   </si>
   <si>
     <t xml:space="preserve">link_spanish</t>
   </si>
   <si>
-    <t xml:space="preserve">**[Documento de política de privacidad](https://drive.google.com/a/upf.edu/file/d/1_LqPgWan5iR3eLphjUcVX-6o4VtzLx73/view?usp=sharing)**</t>
+    <t xml:space="preserve">**[Política de privacidad](https://www.upf.edu/web/cbclab/politica-privacitat)**</t>
   </si>
   <si>
     <t xml:space="preserve">link_english</t>
   </si>
   <si>
-    <t xml:space="preserve">**[Privacy policy document](https://drive.google.com/a/upf.edu/file/d/1YVnflAzAbQYFxppyVFn54CrXlx2PuDEr/view?usp=sharing)**</t>
+    <t xml:space="preserve">**[Privacy policy](https://www.upf.edu/web/cbclab/politica-privacitat)**</t>
   </si>
   <si>
     <t xml:space="preserve">check  </t>
@@ -270,20 +270,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -481,282 +485,286 @@
   </sheetPr>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="3"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="243" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" s="0" t="s">
+      <c r="D2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="0" t="n">
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="243" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" s="0" t="s">
+      <c r="D3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="0" t="n">
+      <c r="H3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="222.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="0" t="s">
+      <c r="D4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="101.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="H4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="0" t="s">
+      <c r="D5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="0" t="n">
+      <c r="H5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="121.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="0" t="s">
+      <c r="D6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="0" t="n">
+      <c r="H6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="101.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="0" t="s">
+      <c r="D7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="0" t="n">
+      <c r="H7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="384.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="0" t="n">
+      <c r="H8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="0" t="n">
+      <c r="H9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="0" t="n">
+      <c r="D10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" s="0" t="n">
+      <c r="D11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="1" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="141.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="0" t="n">
+      <c r="H12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="1" t="n">
         <v>7</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" display="https://www.upf.edu/web/cbclab/politica-privacitat"/>
+    <hyperlink ref="C6" r:id="rId2" display="https://www.upf.edu/web/cbclab/politica-privacitat"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -780,17 +788,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28125" defaultRowHeight="20.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -819,87 +827,87 @@
   <sheetFormatPr defaultColWidth="20" defaultRowHeight="20.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>